<commit_message>
Update for Fri Nov  8 16:33:57 2019
</commit_message>
<xml_diff>
--- a/distros/E/Excel-Writer-XLSX/t/regression/xlsx_files/image06.xlsx
+++ b/distros/E/Excel-Writer-XLSX/t/regression/xlsx_files/image06.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="480" yWindow="270" windowWidth="15855" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -92,24 +92,24 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="46335488"/>
-        <c:axId val="46364544"/>
+        <c:axId val="87089152"/>
+        <c:axId val="87093632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="46335488"/>
+        <c:axId val="87089152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="l"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46364544"/>
+        <c:crossAx val="87093632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="46364544"/>
+        <c:axId val="87093632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -117,7 +117,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="46335488"/>
+        <c:crossAx val="87089152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -138,6 +138,44 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="red.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3048000" y="190500"/>
+          <a:ext cx="304800" cy="304800"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -153,7 +191,7 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -162,48 +200,10 @@
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2" descr="red.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="3048000" y="190500"/>
-          <a:ext cx="304800" cy="304800"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>

</xml_diff>